<commit_message>
Updated to calculate Wing Area
</commit_message>
<xml_diff>
--- a/RC Physical Model/Measurements/Measurements_Small_Scale_F16.xlsx
+++ b/RC Physical Model/Measurements/Measurements_Small_Scale_F16.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Camden\Desktop\Spring 2021\ECE 413\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BC46784-D4D7-47D6-9226-F402CB32460A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8252354C-C896-40E5-9368-DF810D4BC9B6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25395" yWindow="5430" windowWidth="21600" windowHeight="11385" xr2:uid="{B12440C0-934D-46DA-BFA5-1E08A9198AD1}"/>
+    <workbookView xWindow="735" yWindow="855" windowWidth="21600" windowHeight="11385" xr2:uid="{B12440C0-934D-46DA-BFA5-1E08A9198AD1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="42">
   <si>
     <t>Item to Measure</t>
   </si>
@@ -79,12 +79,6 @@
     <t>B</t>
   </si>
   <si>
-    <t>Inches</t>
-  </si>
-  <si>
-    <t>Center of Gravity x coord</t>
-  </si>
-  <si>
     <t>Ixx</t>
   </si>
   <si>
@@ -107,9 +101,6 @@
   </si>
   <si>
     <t>lbs</t>
-  </si>
-  <si>
-    <t>XCGR</t>
   </si>
   <si>
     <t>AXX</t>
@@ -598,8 +589,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9CD20E2-9C8D-4584-ABE5-94254D9DC799}">
   <dimension ref="A1:H40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -622,10 +613,10 @@
         <v>3</v>
       </c>
       <c r="C1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -636,7 +627,11 @@
         <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>24</v>
+        <v>21</v>
+      </c>
+      <c r="D2">
+        <f>(B14*B15)+(((B17-B15)*B14)*0.5)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -650,29 +645,18 @@
         <v>2</v>
       </c>
       <c r="D3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C4" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C5" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D5" t="e">
         <f>H28</f>
@@ -681,13 +665,13 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B6" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C6" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D6" t="e">
         <f t="shared" ref="D6:D7" si="0">H29</f>
@@ -696,13 +680,13 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" t="s">
         <v>11</v>
-      </c>
-      <c r="B7" t="s">
-        <v>20</v>
-      </c>
-      <c r="C7" t="s">
-        <v>13</v>
       </c>
       <c r="D7" t="e">
         <f t="shared" si="0"/>
@@ -711,29 +695,29 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B8" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C8" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B9" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C9" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -743,15 +727,15 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B13" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -761,40 +745,40 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C22" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B22" s="1" t="s">
+      <c r="D22" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C22" s="1" t="s">
+      <c r="E22" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G22" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D22" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="G22" s="1" t="s">
-        <v>38</v>
-      </c>
       <c r="H22" s="1" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
@@ -809,7 +793,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="H23" s="1" t="e">
         <f>((D9*9.8*B23/(4*3.14^2))*E26^2)-(D9*9.8*B23^2)/9.8</f>
@@ -828,7 +812,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="H24" s="1" t="e">
         <f>((D9*9.8*B23/(4*3.14^2))*E33^2)-(D9*9.8*B23^2)/9.8</f>
@@ -847,7 +831,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="H25" s="3" t="e">
         <f>((D9*9.8*B23/(4*3.14^2))*E40^2)-(D9*9.8*B23^2)/9.8</f>
@@ -856,7 +840,7 @@
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
@@ -870,18 +854,18 @@
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="G27" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="H28" s="1" t="e">
         <f>H23*1.3558179619</f>
@@ -890,22 +874,22 @@
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C29" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B29" s="1" t="s">
+      <c r="D29" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C29" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="D29" s="1" t="s">
-        <v>36</v>
-      </c>
       <c r="E29" s="1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="H29" s="1" t="e">
         <f>H24*1.3558179619</f>
@@ -924,7 +908,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="H30" s="1" t="e">
         <f>H25*1.3558179619</f>
@@ -957,7 +941,7 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
@@ -969,24 +953,24 @@
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C36" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B36" s="1" t="s">
+      <c r="D36" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C36" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="D36" s="1" t="s">
-        <v>36</v>
-      </c>
       <c r="E36" s="1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
@@ -1027,7 +1011,7 @@
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>

</xml_diff>